<commit_message>
Add China-linked deals: Kingdee, SenseTime, Huawei, Dahua, G42 divestments
Addresses gap in China coverage. Added 7 China-linked deals across all funds:
- QIA: Kingdee International $200M stake (Shenzhen)
- PIF: Huawei Cloud MOU, SenseTime/SCAI $776M JV, Dahua/AIVisio $200M JV,
  $50B MOU with 6 Chinese banks
- ADIA/G42: ByteDance/xFusion/Honor divestment (US pressure),
  42XFund transfer to Lunate (JD.com, ByteDance)
Also added MGX-Silver Lake Altera 51% stake ($8.75B semiconductor deal)
and PIF-Google Cloud $10B AI Hub. Total: 52 deals.

https://claude.ai/code/session_0171mdbGQcfY5KsoC6NY57bZ
</commit_message>
<xml_diff>
--- a/output/SWF_AI_Semiconductor_Deals.xlsx
+++ b/output/SWF_AI_Semiconductor_Deals.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SWF AI-Semiconductor Deals" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SWF AI-Semiconductor Deals'!$A$4:$G$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SWF AI-Semiconductor Deals'!$A$4:$G$56</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -545,7 +545,7 @@
     <row r="2" ht="22" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Sources: Reuters, Bloomberg, MEI (M. Soliman), Global SWF, The National News, AGBI, Official Fund Newsrooms | Generated: 2026-02-09 21:21</t>
+          <t>Sources: Reuters, Bloomberg, MEI (M. Soliman), Global SWF, The National News, AGBI, Official Fund Newsrooms | Generated: 2026-02-13 19:10</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
     <row r="8" ht="22" customHeight="1">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>2024-05-13</t>
+          <t>2023-12-10</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr">
@@ -710,34 +710,34 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>Ardian Semiconductor</t>
+          <t>Kingdee International Software</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>Semiconductors</t>
+          <t>AI/ML Platform</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>Europe (France)</t>
+          <t>China (Shenzhen)</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>Fund (Anchor investor)</t>
+          <t>Stake (4.26%, $200M)</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>Bloomberg / QIA Newsroom</t>
+          <t>China Daily / Reuters</t>
         </is>
       </c>
     </row>
     <row r="9" ht="22" customHeight="1">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2024-05-13</t>
         </is>
       </c>
       <c r="B9" s="4" t="inlineStr">
@@ -747,34 +747,34 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>xAI (Elon Musk)</t>
+          <t>Ardian Semiconductor</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>Semiconductors</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>Europe (France)</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>Fund (Series C, $6B round)</t>
+          <t>Fund (Anchor investor)</t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>Reuters / AGBI</t>
+          <t>Bloomberg / QIA Newsroom</t>
         </is>
       </c>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>2024-11-19</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="B10" s="4" t="inlineStr">
@@ -784,12 +784,12 @@
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>Cresta AI</t>
+          <t>xAI (Elon Musk)</t>
         </is>
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>AI/ML Platform</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -799,19 +799,19 @@
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>Fund (Series D co-lead, $125M)</t>
+          <t>Fund (Series C, $6B round)</t>
         </is>
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>Bloomberg / AGBI</t>
+          <t>Reuters / AGBI</t>
         </is>
       </c>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>2025-01-15</t>
+          <t>2024-11-19</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>Databricks</t>
+          <t>Cresta AI</t>
         </is>
       </c>
       <c r="D11" s="4" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>Fund ($15B round follow-on)</t>
+          <t>Fund (Series D co-lead, $125M)</t>
         </is>
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>QIA Newsroom / Reuters</t>
+          <t>Bloomberg / AGBI</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>Instabase</t>
+          <t>Databricks</t>
         </is>
       </c>
       <c r="D12" s="4" t="inlineStr">
@@ -873,19 +873,19 @@
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>Fund (Series D lead, $100M)</t>
+          <t>Fund ($15B round follow-on)</t>
         </is>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Bloomberg / The National News</t>
+          <t>QIA Newsroom / Reuters</t>
         </is>
       </c>
     </row>
     <row r="13" ht="22" customHeight="1">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
@@ -895,12 +895,12 @@
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>xAI (Elon Musk)</t>
+          <t>Instabase</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>AI/ML Platform</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -910,19 +910,19 @@
       </c>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>Fund (Series E, $20B round)</t>
+          <t>Fund (Series D lead, $100M)</t>
         </is>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>Reuters / AGBI</t>
+          <t>Bloomberg / The National News</t>
         </is>
       </c>
     </row>
     <row r="14" ht="22" customHeight="1">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-05-01</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
@@ -932,34 +932,34 @@
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>Blue Owl Capital</t>
+          <t>xAI (Elon Musk)</t>
         </is>
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>Data Centers</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>US (Global)</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>JV ($3B+ digital infra platform)</t>
+          <t>Fund (Series E, $20B round)</t>
         </is>
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>Bloomberg / QIA Newsroom</t>
+          <t>Reuters / AGBI</t>
         </is>
       </c>
     </row>
     <row r="15" ht="22" customHeight="1">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
@@ -969,34 +969,34 @@
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Qai (QIA subsidiary) / Brookfield</t>
+          <t>Blue Owl Capital</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>Data Centers</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>Qatar (Global)</t>
+          <t>US (Global)</t>
         </is>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>JV ($20B AI infra partnership)</t>
+          <t>JV ($3B+ digital infra platform)</t>
         </is>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>QIA Newsroom / Reuters</t>
+          <t>Bloomberg / QIA Newsroom</t>
         </is>
       </c>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>2025-06-01</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
@@ -1006,34 +1006,34 @@
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>Anthropic</t>
+          <t>Qai (QIA subsidiary) / Brookfield</t>
         </is>
       </c>
       <c r="D16" s="4" t="inlineStr">
         <is>
-          <t>AI Models/Research</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>Qatar (Global)</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>Fund ($13B round participation)</t>
+          <t>JV ($20B AI infra partnership)</t>
         </is>
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>Bloomberg / The National News</t>
+          <t>QIA Newsroom / Reuters</t>
         </is>
       </c>
     </row>
     <row r="17" ht="22" customHeight="1">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-06-01</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
@@ -1043,27 +1043,27 @@
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>Alice &amp; Bob (with Bpifrance)</t>
+          <t>Anthropic</t>
         </is>
       </c>
       <c r="D17" s="4" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>AI Models/Research</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>JV (Quantum computing investment)</t>
+          <t>Fund ($13B round participation)</t>
         </is>
       </c>
       <c r="G17" s="4" t="inlineStr">
         <is>
-          <t>AGBI / Global SWF</t>
+          <t>Bloomberg / The National News</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
     <row r="20" ht="22" customHeight="1">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>2024-02-20</t>
+          <t>2022-12-09</t>
         </is>
       </c>
       <c r="B20" s="5" t="inlineStr">
@@ -1154,34 +1154,34 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>SoftBank Group (via Alat)</t>
+          <t>Huawei Cloud</t>
         </is>
       </c>
       <c r="D20" s="5" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>AI Cloud Computing</t>
         </is>
       </c>
       <c r="E20" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>China / Saudi Arabia</t>
         </is>
       </c>
       <c r="F20" s="5" t="inlineStr">
         <is>
-          <t>JV ($150M robot mfg. hub)</t>
+          <t>MOU (Cloud &amp; AI infra buildout)</t>
         </is>
       </c>
       <c r="G20" s="5" t="inlineStr">
         <is>
-          <t>SoftBank / Arab News</t>
+          <t>China Daily / Bloomberg</t>
         </is>
       </c>
     </row>
     <row r="21" ht="22" customHeight="1">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>2024-03-01</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="B21" s="5" t="inlineStr">
@@ -1191,34 +1191,34 @@
       </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
-          <t>Amazon Web Services (AWS)</t>
+          <t>SenseTime (via SCAI JV)</t>
         </is>
       </c>
       <c r="D21" s="5" t="inlineStr">
         <is>
-          <t>AI Cloud Computing</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E21" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>China / Saudi Arabia</t>
         </is>
       </c>
       <c r="F21" s="5" t="inlineStr">
         <is>
-          <t>MOU ($5.3B AI Zone)</t>
+          <t>JV ($776M AI ecosystem dev.)</t>
         </is>
       </c>
       <c r="G21" s="5" t="inlineStr">
         <is>
-          <t>Reuters / Bloomberg</t>
+          <t>Arab News / Bloomberg</t>
         </is>
       </c>
     </row>
     <row r="22" ht="22" customHeight="1">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2024-02-20</t>
         </is>
       </c>
       <c r="B22" s="5" t="inlineStr">
@@ -1228,34 +1228,34 @@
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
-          <t>Groq (via Aramco Digital)</t>
+          <t>Dahua Technology (via Alat/AIVisio)</t>
         </is>
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>AI Chips</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E22" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia (Dammam)</t>
+          <t>China / Saudi Arabia</t>
         </is>
       </c>
       <c r="F22" s="5" t="inlineStr">
         <is>
-          <t>JV (AI inference datacenter)</t>
+          <t>JV ($200M AIoT mfg. hub)</t>
         </is>
       </c>
       <c r="G22" s="5" t="inlineStr">
         <is>
-          <t>Reuters / The National News</t>
+          <t>Arab News / Euronews</t>
         </is>
       </c>
     </row>
     <row r="23" ht="22" customHeight="1">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>2025-02-10</t>
+          <t>2024-02-20</t>
         </is>
       </c>
       <c r="B23" s="5" t="inlineStr">
@@ -1265,34 +1265,34 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>Groq / Aramco Digital</t>
+          <t>SoftBank Group (via Alat)</t>
         </is>
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>AI Inference</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E23" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia (Dammam)</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="F23" s="5" t="inlineStr">
         <is>
-          <t>Fund ($1.5B expansion)</t>
+          <t>JV ($150M robot mfg. hub)</t>
         </is>
       </c>
       <c r="G23" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / MEI</t>
+          <t>SoftBank / Arab News</t>
         </is>
       </c>
     </row>
     <row r="24" ht="22" customHeight="1">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>2025-02-10</t>
+          <t>2024-03-01</t>
         </is>
       </c>
       <c r="B24" s="5" t="inlineStr">
@@ -1302,12 +1302,12 @@
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>Databricks (LEAP 2025)</t>
+          <t>Amazon Web Services (AWS)</t>
         </is>
       </c>
       <c r="D24" s="5" t="inlineStr">
         <is>
-          <t>AI/ML Platform</t>
+          <t>AI Cloud Computing</t>
         </is>
       </c>
       <c r="E24" s="5" t="inlineStr">
@@ -1317,19 +1317,19 @@
       </c>
       <c r="F24" s="5" t="inlineStr">
         <is>
-          <t>MOU ($300M PaaS commitment)</t>
+          <t>MOU ($5.3B AI Zone)</t>
         </is>
       </c>
       <c r="G24" s="5" t="inlineStr">
         <is>
-          <t>Arab News / LEAP</t>
+          <t>Reuters / Bloomberg</t>
         </is>
       </c>
     </row>
     <row r="25" ht="22" customHeight="1">
       <c r="A25" s="5" t="inlineStr">
         <is>
-          <t>2025-02-10</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="B25" s="5" t="inlineStr">
@@ -1339,34 +1339,34 @@
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>Salesforce (LEAP 2025)</t>
+          <t>6 Chinese banks (ICBC, BoC, CCB, etc.)</t>
         </is>
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>AI Cloud Computing</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>China / Saudi Arabia</t>
         </is>
       </c>
       <c r="F25" s="5" t="inlineStr">
         <is>
-          <t>MOU ($500M Hyperforce)</t>
+          <t>MOU ($50B framework for tech/infra)</t>
         </is>
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
-          <t>Arab News / LEAP</t>
+          <t>Al-Monitor / Reuters</t>
         </is>
       </c>
     </row>
     <row r="26" ht="22" customHeight="1">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>2025-02-10</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="B26" s="5" t="inlineStr">
@@ -1376,34 +1376,34 @@
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>Lenovo (via Alat)</t>
+          <t>Groq (via Aramco Digital)</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>AI Chips</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Saudi Arabia (Dammam)</t>
         </is>
       </c>
       <c r="F26" s="5" t="inlineStr">
         <is>
-          <t>JV ($2B mfg. &amp; regional HQ)</t>
+          <t>JV (AI inference datacenter)</t>
         </is>
       </c>
       <c r="G26" s="5" t="inlineStr">
         <is>
-          <t>Arab News / LEAP</t>
+          <t>Reuters / The National News</t>
         </is>
       </c>
     </row>
     <row r="27" ht="22" customHeight="1">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>2025-Q2</t>
+          <t>2025-02-10</t>
         </is>
       </c>
       <c r="B27" s="5" t="inlineStr">
@@ -1413,34 +1413,34 @@
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>Arm Holdings</t>
+          <t>Groq / Aramco Digital</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>Semiconductors</t>
+          <t>AI Inference</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>US / UK</t>
+          <t>Saudi Arabia (Dammam)</t>
         </is>
       </c>
       <c r="F27" s="5" t="inlineStr">
         <is>
-          <t>Stake (doubled holding)</t>
+          <t>Fund ($1.5B expansion)</t>
         </is>
       </c>
       <c r="G27" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / Arab News (SEC 13F)</t>
+          <t>Bloomberg / MEI</t>
         </is>
       </c>
     </row>
     <row r="28" ht="22" customHeight="1">
       <c r="A28" s="5" t="inlineStr">
         <is>
-          <t>2025-Q1</t>
+          <t>2025-02-10</t>
         </is>
       </c>
       <c r="B28" s="5" t="inlineStr">
@@ -1450,34 +1450,34 @@
       </c>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>ASML Holding</t>
+          <t>Databricks (LEAP 2025)</t>
         </is>
       </c>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>Semiconductor Equipment</t>
+          <t>AI/ML Platform</t>
         </is>
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="F28" s="5" t="inlineStr">
         <is>
-          <t>Stake (options position)</t>
+          <t>MOU ($300M PaaS commitment)</t>
         </is>
       </c>
       <c r="G28" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / Arab News (SEC 13F)</t>
+          <t>Arab News / LEAP</t>
         </is>
       </c>
     </row>
     <row r="29" ht="22" customHeight="1">
       <c r="A29" s="5" t="inlineStr">
         <is>
-          <t>2025-Q2</t>
+          <t>2025-02-10</t>
         </is>
       </c>
       <c r="B29" s="5" t="inlineStr">
@@ -1487,34 +1487,34 @@
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>Analog Devices</t>
+          <t>Salesforce (LEAP 2025)</t>
         </is>
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>Semiconductors</t>
+          <t>AI Cloud Computing</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="F29" s="5" t="inlineStr">
         <is>
-          <t>Stake (new position)</t>
+          <t>MOU ($500M Hyperforce)</t>
         </is>
       </c>
       <c r="G29" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / Arab News (SEC 13F)</t>
+          <t>Arab News / LEAP</t>
         </is>
       </c>
     </row>
     <row r="30" ht="22" customHeight="1">
       <c r="A30" s="5" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-02-10</t>
         </is>
       </c>
       <c r="B30" s="5" t="inlineStr">
@@ -1524,34 +1524,34 @@
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
-          <t>NVIDIA (via HUMAIN)</t>
+          <t>Lenovo (via Alat)</t>
         </is>
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
-          <t>AI Chips</t>
+          <t>AI Infrastructure</t>
         </is>
       </c>
       <c r="E30" s="5" t="inlineStr">
         <is>
-          <t>US / Saudi Arabia</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="F30" s="5" t="inlineStr">
         <is>
-          <t>MOU (18,000 GB300 chips)</t>
+          <t>JV ($2B mfg. &amp; regional HQ)</t>
         </is>
       </c>
       <c r="G30" s="5" t="inlineStr">
         <is>
-          <t>Reuters / Bloomberg / NVIDIA</t>
+          <t>Arab News / LEAP</t>
         </is>
       </c>
     </row>
     <row r="31" ht="22" customHeight="1">
       <c r="A31" s="5" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-Q2</t>
         </is>
       </c>
       <c r="B31" s="5" t="inlineStr">
@@ -1561,34 +1561,34 @@
       </c>
       <c r="C31" s="5" t="inlineStr">
         <is>
-          <t>AMD (via HUMAIN)</t>
+          <t>Arm Holdings</t>
         </is>
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>AI Chips</t>
+          <t>Semiconductors</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr">
         <is>
-          <t>US / Saudi Arabia</t>
+          <t>US / UK</t>
         </is>
       </c>
       <c r="F31" s="5" t="inlineStr">
         <is>
-          <t>JV ($10B AI infra, 500MW)</t>
+          <t>Stake (doubled holding)</t>
         </is>
       </c>
       <c r="G31" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / The National News</t>
+          <t>Bloomberg / Arab News (SEC 13F)</t>
         </is>
       </c>
     </row>
     <row r="32" ht="22" customHeight="1">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-Q1</t>
         </is>
       </c>
       <c r="B32" s="5" t="inlineStr">
@@ -1598,34 +1598,34 @@
       </c>
       <c r="C32" s="5" t="inlineStr">
         <is>
-          <t>HUMAIN launch (PIF subsidiary)</t>
+          <t>ASML Holding</t>
         </is>
       </c>
       <c r="D32" s="5" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>Semiconductor Equipment</t>
         </is>
       </c>
       <c r="E32" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia (Global)</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="F32" s="5" t="inlineStr">
         <is>
-          <t>Fund (National AI champion)</t>
+          <t>Stake (options position)</t>
         </is>
       </c>
       <c r="G32" s="5" t="inlineStr">
         <is>
-          <t>PIF Official / Reuters</t>
+          <t>Bloomberg / Arab News (SEC 13F)</t>
         </is>
       </c>
     </row>
     <row r="33" ht="22" customHeight="1">
       <c r="A33" s="5" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-Q2</t>
         </is>
       </c>
       <c r="B33" s="5" t="inlineStr">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="C33" s="5" t="inlineStr">
         <is>
-          <t>Qualcomm (via HUMAIN)</t>
+          <t>Analog Devices</t>
         </is>
       </c>
       <c r="D33" s="5" t="inlineStr">
@@ -1645,24 +1645,24 @@
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
-          <t>US / Saudi Arabia</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F33" s="5" t="inlineStr">
         <is>
-          <t>MOU (Design center partnership)</t>
+          <t>Stake (new position)</t>
         </is>
       </c>
       <c r="G33" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / Arab News</t>
+          <t>Bloomberg / Arab News (SEC 13F)</t>
         </is>
       </c>
     </row>
     <row r="34" ht="22" customHeight="1">
       <c r="A34" s="5" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="B34" s="5" t="inlineStr">
@@ -1672,34 +1672,34 @@
       </c>
       <c r="C34" s="5" t="inlineStr">
         <is>
-          <t>Blackstone / AirTrunk (via HUMAIN)</t>
+          <t>NVIDIA (via HUMAIN)</t>
         </is>
       </c>
       <c r="D34" s="5" t="inlineStr">
         <is>
-          <t>Data Centers</t>
+          <t>AI Chips</t>
         </is>
       </c>
       <c r="E34" s="5" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>US / Saudi Arabia</t>
         </is>
       </c>
       <c r="F34" s="5" t="inlineStr">
         <is>
-          <t>JV ($3B data center campus)</t>
+          <t>MOU (18,000 GB300 chips)</t>
         </is>
       </c>
       <c r="G34" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / Blackstone</t>
+          <t>Reuters / Bloomberg / NVIDIA</t>
         </is>
       </c>
     </row>
     <row r="35" ht="22" customHeight="1">
       <c r="A35" s="5" t="inlineStr">
         <is>
-          <t>2025-11-01</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="B35" s="5" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="C35" s="5" t="inlineStr">
         <is>
-          <t>NVIDIA (expanded, via HUMAIN)</t>
+          <t>AMD (via HUMAIN)</t>
         </is>
       </c>
       <c r="D35" s="5" t="inlineStr">
@@ -1724,19 +1724,19 @@
       </c>
       <c r="F35" s="5" t="inlineStr">
         <is>
-          <t>MOU (600K chips over 3 years)</t>
+          <t>JV ($10B AI infra, 500MW)</t>
         </is>
       </c>
       <c r="G35" s="5" t="inlineStr">
         <is>
-          <t>Reuters / Bloomberg</t>
+          <t>Bloomberg / The National News</t>
         </is>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1">
       <c r="A36" s="5" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-05-01</t>
         </is>
       </c>
       <c r="B36" s="5" t="inlineStr">
@@ -1746,293 +1746,293 @@
       </c>
       <c r="C36" s="5" t="inlineStr">
         <is>
-          <t>AMD / Cisco (via HUMAIN)</t>
+          <t>Qualcomm (via HUMAIN)</t>
         </is>
       </c>
       <c r="D36" s="5" t="inlineStr">
         <is>
-          <t>AI Infrastructure</t>
+          <t>Semiconductors</t>
         </is>
       </c>
       <c r="E36" s="5" t="inlineStr">
         <is>
-          <t>US / Saudi Arabia (Global)</t>
+          <t>US / Saudi Arabia</t>
         </is>
       </c>
       <c r="F36" s="5" t="inlineStr">
         <is>
-          <t>JV (1GW AI infra by 2030)</t>
+          <t>MOU (Design center partnership)</t>
         </is>
       </c>
       <c r="G36" s="5" t="inlineStr">
         <is>
-          <t>Bloomberg / Cisco Newsroom</t>
+          <t>Bloomberg / Arab News</t>
         </is>
       </c>
     </row>
     <row r="37" ht="22" customHeight="1">
       <c r="A37" s="5" t="inlineStr">
         <is>
+          <t>2025-10-28</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="inlineStr">
+        <is>
+          <t>PIF</t>
+        </is>
+      </c>
+      <c r="C37" s="5" t="inlineStr">
+        <is>
+          <t>Blackstone / AirTrunk (via HUMAIN)</t>
+        </is>
+      </c>
+      <c r="D37" s="5" t="inlineStr">
+        <is>
+          <t>Data Centers</t>
+        </is>
+      </c>
+      <c r="E37" s="5" t="inlineStr">
+        <is>
+          <t>Saudi Arabia</t>
+        </is>
+      </c>
+      <c r="F37" s="5" t="inlineStr">
+        <is>
+          <t>JV ($3B data center campus)</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Bloomberg / Blackstone</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="22" customHeight="1">
+      <c r="A38" s="5" t="inlineStr">
+        <is>
           <t>2025-11-01</t>
         </is>
       </c>
-      <c r="B37" s="5" t="inlineStr">
+      <c r="B38" s="5" t="inlineStr">
         <is>
           <t>PIF</t>
         </is>
       </c>
-      <c r="C37" s="5" t="inlineStr">
-        <is>
-          <t>AWS (via HUMAIN, expanded)</t>
-        </is>
-      </c>
-      <c r="D37" s="5" t="inlineStr">
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>NVIDIA (expanded, via HUMAIN)</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="inlineStr">
+        <is>
+          <t>AI Chips</t>
+        </is>
+      </c>
+      <c r="E38" s="5" t="inlineStr">
+        <is>
+          <t>US / Saudi Arabia</t>
+        </is>
+      </c>
+      <c r="F38" s="5" t="inlineStr">
+        <is>
+          <t>MOU (600K chips over 3 years)</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Reuters / Bloomberg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="22" customHeight="1">
+      <c r="A39" s="5" t="inlineStr">
+        <is>
+          <t>2025-11-19</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="inlineStr">
+        <is>
+          <t>PIF</t>
+        </is>
+      </c>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>AMD / Cisco (via HUMAIN)</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr">
+        <is>
+          <t>AI Infrastructure</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="inlineStr">
+        <is>
+          <t>US / Saudi Arabia (Global)</t>
+        </is>
+      </c>
+      <c r="F39" s="5" t="inlineStr">
+        <is>
+          <t>JV (1GW AI infra by 2030)</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Bloomberg / Cisco Newsroom</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="22" customHeight="1">
+      <c r="A40" s="5" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="inlineStr">
+        <is>
+          <t>PIF</t>
+        </is>
+      </c>
+      <c r="C40" s="5" t="inlineStr">
+        <is>
+          <t>Google Cloud (via HUMAIN)</t>
+        </is>
+      </c>
+      <c r="D40" s="5" t="inlineStr">
         <is>
           <t>AI Cloud Computing</t>
         </is>
       </c>
-      <c r="E37" s="5" t="inlineStr">
-        <is>
-          <t>Saudi Arabia (Riyadh)</t>
-        </is>
-      </c>
-      <c r="F37" s="5" t="inlineStr">
-        <is>
-          <t>MOU (150K NVIDIA GPUs in AI Zone)</t>
-        </is>
-      </c>
-      <c r="G37" s="5" t="inlineStr">
-        <is>
-          <t>Bloomberg / Reuters</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" ht="22" customHeight="1">
-      <c r="A38" s="6" t="inlineStr">
+      <c r="E40" s="5" t="inlineStr">
+        <is>
+          <t>US / Saudi Arabia</t>
+        </is>
+      </c>
+      <c r="F40" s="5" t="inlineStr">
+        <is>
+          <t>JV ($10B AI Hub partnership)</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Google Cloud / Bloomberg</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="22" customHeight="1">
+      <c r="A41" s="6" t="inlineStr">
         <is>
           <t>2023-11-01</t>
         </is>
       </c>
-      <c r="B38" s="6" t="inlineStr">
+      <c r="B41" s="6" t="inlineStr">
         <is>
           <t>ADIA</t>
         </is>
       </c>
-      <c r="C38" s="6" t="inlineStr">
+      <c r="C41" s="6" t="inlineStr">
         <is>
           <t>Landmark Dividend / DigitalBridge</t>
         </is>
       </c>
-      <c r="D38" s="6" t="inlineStr">
+      <c r="D41" s="6" t="inlineStr">
         <is>
           <t>Digital Infrastructure</t>
         </is>
       </c>
-      <c r="E38" s="6" t="inlineStr">
+      <c r="E41" s="6" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F38" s="6" t="inlineStr">
+      <c r="F41" s="6" t="inlineStr">
         <is>
           <t>Stake (40% acquisition)</t>
         </is>
       </c>
-      <c r="G38" s="6" t="inlineStr">
+      <c r="G41" s="6" t="inlineStr">
         <is>
           <t>Bloomberg / DigitalBridge</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="22" customHeight="1">
-      <c r="A39" s="7" t="inlineStr">
-        <is>
-          <t>2024-03-01</t>
-        </is>
-      </c>
-      <c r="B39" s="7" t="inlineStr">
-        <is>
-          <t>MGX/Mubadala</t>
-        </is>
-      </c>
-      <c r="C39" s="7" t="inlineStr">
-        <is>
-          <t>MGX launch (Mubadala + G42)</t>
-        </is>
-      </c>
-      <c r="D39" s="7" t="inlineStr">
+    <row r="42" ht="22" customHeight="1">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="B42" s="6" t="inlineStr">
+        <is>
+          <t>ADIA</t>
+        </is>
+      </c>
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>G42 divests ByteDance/xFusion/Honor</t>
+        </is>
+      </c>
+      <c r="D42" s="6" t="inlineStr">
         <is>
           <t>AI Infrastructure</t>
         </is>
       </c>
-      <c r="E39" s="7" t="inlineStr">
-        <is>
-          <t>UAE (Global)</t>
-        </is>
-      </c>
-      <c r="F39" s="7" t="inlineStr">
-        <is>
-          <t>Fund ($100B AI investment vehicle)</t>
-        </is>
-      </c>
-      <c r="G39" s="7" t="inlineStr">
-        <is>
-          <t>Bloomberg / The National News</t>
-        </is>
-      </c>
-    </row>
-    <row r="40" ht="22" customHeight="1">
-      <c r="A40" s="7" t="inlineStr">
-        <is>
-          <t>2024-09-17</t>
-        </is>
-      </c>
-      <c r="B40" s="7" t="inlineStr">
-        <is>
-          <t>MGX/Mubadala</t>
-        </is>
-      </c>
-      <c r="C40" s="7" t="inlineStr">
-        <is>
-          <t>BlackRock / Microsoft / GIP</t>
-        </is>
-      </c>
-      <c r="D40" s="7" t="inlineStr">
+      <c r="E42" s="6" t="inlineStr">
+        <is>
+          <t>China (Divestment)</t>
+        </is>
+      </c>
+      <c r="F42" s="6" t="inlineStr">
+        <is>
+          <t>Stake (Divestment, US pressure)</t>
+        </is>
+      </c>
+      <c r="G42" s="6" t="inlineStr">
+        <is>
+          <t>NYT / Financial Times</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="22" customHeight="1">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>ADIA</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>G42-Microsoft ($1.5B, China exit cond.)</t>
+        </is>
+      </c>
+      <c r="D43" s="6" t="inlineStr">
         <is>
           <t>AI Infrastructure</t>
         </is>
       </c>
-      <c r="E40" s="7" t="inlineStr">
-        <is>
-          <t>US (Global)</t>
-        </is>
-      </c>
-      <c r="F40" s="7" t="inlineStr">
-        <is>
-          <t>JV ($30B equity, $100B total GAIIP)</t>
-        </is>
-      </c>
-      <c r="G40" s="7" t="inlineStr">
-        <is>
-          <t>Bloomberg / Microsoft / BlackRock</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="22" customHeight="1">
-      <c r="A41" s="7" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="B41" s="7" t="inlineStr">
-        <is>
-          <t>MGX/Mubadala</t>
-        </is>
-      </c>
-      <c r="C41" s="7" t="inlineStr">
-        <is>
-          <t>OpenAI</t>
-        </is>
-      </c>
-      <c r="D41" s="7" t="inlineStr">
-        <is>
-          <t>AI Models/Research</t>
-        </is>
-      </c>
-      <c r="E41" s="7" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F41" s="7" t="inlineStr">
-        <is>
-          <t>Fund ($6.6B round, $157B val.)</t>
-        </is>
-      </c>
-      <c r="G41" s="7" t="inlineStr">
-        <is>
-          <t>Bloomberg / Reuters</t>
-        </is>
-      </c>
-    </row>
-    <row r="42" ht="22" customHeight="1">
-      <c r="A42" s="7" t="inlineStr">
-        <is>
-          <t>2024-11-01</t>
-        </is>
-      </c>
-      <c r="B42" s="7" t="inlineStr">
-        <is>
-          <t>MGX/Mubadala</t>
-        </is>
-      </c>
-      <c r="C42" s="7" t="inlineStr">
-        <is>
-          <t>xAI (Elon Musk)</t>
-        </is>
-      </c>
-      <c r="D42" s="7" t="inlineStr">
-        <is>
-          <t>AI Infrastructure</t>
-        </is>
-      </c>
-      <c r="E42" s="7" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F42" s="7" t="inlineStr">
-        <is>
-          <t>Fund (Series C, $6B round)</t>
-        </is>
-      </c>
-      <c r="G42" s="7" t="inlineStr">
-        <is>
-          <t>Reuters / AGBI</t>
-        </is>
-      </c>
-    </row>
-    <row r="43" ht="22" customHeight="1">
-      <c r="A43" s="7" t="inlineStr">
-        <is>
-          <t>2024-11-01</t>
-        </is>
-      </c>
-      <c r="B43" s="7" t="inlineStr">
-        <is>
-          <t>MGX/Mubadala</t>
-        </is>
-      </c>
-      <c r="C43" s="7" t="inlineStr">
-        <is>
-          <t>Databricks</t>
-        </is>
-      </c>
-      <c r="D43" s="7" t="inlineStr">
-        <is>
-          <t>AI/ML Platform</t>
-        </is>
-      </c>
-      <c r="E43" s="7" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F43" s="7" t="inlineStr">
-        <is>
-          <t>Fund ($10B round, $62B val.)</t>
-        </is>
-      </c>
-      <c r="G43" s="7" t="inlineStr">
-        <is>
-          <t>Bloomberg / Global SWF</t>
+      <c r="E43" s="6" t="inlineStr">
+        <is>
+          <t>US / UAE</t>
+        </is>
+      </c>
+      <c r="F43" s="6" t="inlineStr">
+        <is>
+          <t>Fund ($1.5B conditioned on China exit)</t>
+        </is>
+      </c>
+      <c r="G43" s="6" t="inlineStr">
+        <is>
+          <t>Bloomberg / Microsoft</t>
         </is>
       </c>
     </row>
     <row r="44" ht="22" customHeight="1">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>2024-11-11</t>
+          <t>2024-07-08</t>
         </is>
       </c>
       <c r="B44" s="6" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="C44" s="6" t="inlineStr">
         <is>
-          <t>Qlik Technologies (with Thoma Bravo)</t>
+          <t>G42 42XFund → Lunate (JD.com, ByteDance)</t>
         </is>
       </c>
       <c r="D44" s="6" t="inlineStr">
@@ -2052,61 +2052,61 @@
       </c>
       <c r="E44" s="6" t="inlineStr">
         <is>
-          <t>US / Sweden</t>
+          <t>China (Restructured)</t>
         </is>
       </c>
       <c r="F44" s="6" t="inlineStr">
         <is>
-          <t>Stake (~$1B minority, $10B val.)</t>
+          <t>Fund (China fund transferred to Lunate)</t>
         </is>
       </c>
       <c r="G44" s="6" t="inlineStr">
         <is>
+          <t>Bloomberg / AGBI</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="22" customHeight="1">
+      <c r="A45" s="7" t="inlineStr">
+        <is>
+          <t>2024-03-01</t>
+        </is>
+      </c>
+      <c r="B45" s="7" t="inlineStr">
+        <is>
+          <t>MGX/Mubadala</t>
+        </is>
+      </c>
+      <c r="C45" s="7" t="inlineStr">
+        <is>
+          <t>MGX launch (Mubadala + G42)</t>
+        </is>
+      </c>
+      <c r="D45" s="7" t="inlineStr">
+        <is>
+          <t>AI Infrastructure</t>
+        </is>
+      </c>
+      <c r="E45" s="7" t="inlineStr">
+        <is>
+          <t>UAE (Global)</t>
+        </is>
+      </c>
+      <c r="F45" s="7" t="inlineStr">
+        <is>
+          <t>Fund ($100B AI investment vehicle)</t>
+        </is>
+      </c>
+      <c r="G45" s="7" t="inlineStr">
+        <is>
           <t>Bloomberg / The National News</t>
-        </is>
-      </c>
-    </row>
-    <row r="45" ht="22" customHeight="1">
-      <c r="A45" s="6" t="inlineStr">
-        <is>
-          <t>2025-01-13</t>
-        </is>
-      </c>
-      <c r="B45" s="6" t="inlineStr">
-        <is>
-          <t>ADIA</t>
-        </is>
-      </c>
-      <c r="C45" s="6" t="inlineStr">
-        <is>
-          <t>AlphaGen / ArcLight Capital</t>
-        </is>
-      </c>
-      <c r="D45" s="6" t="inlineStr">
-        <is>
-          <t>Power Infrastructure</t>
-        </is>
-      </c>
-      <c r="E45" s="6" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F45" s="6" t="inlineStr">
-        <is>
-          <t>Stake ($500M minority, 11GW)</t>
-        </is>
-      </c>
-      <c r="G45" s="6" t="inlineStr">
-        <is>
-          <t>Reuters / Arab News</t>
         </is>
       </c>
     </row>
     <row r="46" ht="22" customHeight="1">
       <c r="A46" s="7" t="inlineStr">
         <is>
-          <t>2025-01-21</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="B46" s="7" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C46" s="7" t="inlineStr">
         <is>
-          <t>OpenAI / SoftBank / Oracle (Stargate)</t>
+          <t>BlackRock / Microsoft / GIP</t>
         </is>
       </c>
       <c r="D46" s="7" t="inlineStr">
@@ -2131,19 +2131,19 @@
       </c>
       <c r="F46" s="7" t="inlineStr">
         <is>
-          <t>JV ($500B AI infra, $7B MGX equity)</t>
+          <t>JV ($30B equity, $100B total GAIIP)</t>
         </is>
       </c>
       <c r="G46" s="7" t="inlineStr">
         <is>
-          <t>Reuters / Bloomberg / MEI</t>
+          <t>Bloomberg / Microsoft / BlackRock</t>
         </is>
       </c>
     </row>
     <row r="47" ht="22" customHeight="1">
       <c r="A47" s="7" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="B47" s="7" t="inlineStr">
@@ -2153,177 +2153,436 @@
       </c>
       <c r="C47" s="7" t="inlineStr">
         <is>
-          <t>NVIDIA / xAI (joined AIP)</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="D47" s="7" t="inlineStr">
         <is>
+          <t>AI Models/Research</t>
+        </is>
+      </c>
+      <c r="E47" s="7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F47" s="7" t="inlineStr">
+        <is>
+          <t>Fund ($6.6B round, $157B val.)</t>
+        </is>
+      </c>
+      <c r="G47" s="7" t="inlineStr">
+        <is>
+          <t>Bloomberg / Reuters</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="22" customHeight="1">
+      <c r="A48" s="7" t="inlineStr">
+        <is>
+          <t>2024-11-01</t>
+        </is>
+      </c>
+      <c r="B48" s="7" t="inlineStr">
+        <is>
+          <t>MGX/Mubadala</t>
+        </is>
+      </c>
+      <c r="C48" s="7" t="inlineStr">
+        <is>
+          <t>xAI (Elon Musk)</t>
+        </is>
+      </c>
+      <c r="D48" s="7" t="inlineStr">
+        <is>
           <t>AI Infrastructure</t>
         </is>
       </c>
-      <c r="E47" s="7" t="inlineStr">
+      <c r="E48" s="7" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F47" s="7" t="inlineStr">
-        <is>
-          <t>JV (AIP expansion with NVIDIA, xAI)</t>
-        </is>
-      </c>
-      <c r="G47" s="7" t="inlineStr">
-        <is>
-          <t>BlackRock / Bloomberg</t>
-        </is>
-      </c>
-    </row>
-    <row r="48" ht="22" customHeight="1">
-      <c r="A48" s="6" t="inlineStr">
-        <is>
-          <t>2025-09-10</t>
-        </is>
-      </c>
-      <c r="B48" s="6" t="inlineStr">
-        <is>
-          <t>ADIA</t>
-        </is>
-      </c>
-      <c r="C48" s="6" t="inlineStr">
-        <is>
-          <t>Vantage Data Centers (with GIC)</t>
-        </is>
-      </c>
-      <c r="D48" s="6" t="inlineStr">
-        <is>
-          <t>Data Centers</t>
-        </is>
-      </c>
-      <c r="E48" s="6" t="inlineStr">
-        <is>
-          <t>Asia-Pacific</t>
-        </is>
-      </c>
-      <c r="F48" s="6" t="inlineStr">
-        <is>
-          <t>Fund ($1.6B APAC platform)</t>
-        </is>
-      </c>
-      <c r="G48" s="6" t="inlineStr">
-        <is>
-          <t>Bloomberg / The National News</t>
+      <c r="F48" s="7" t="inlineStr">
+        <is>
+          <t>Fund (Series C, $6B round)</t>
+        </is>
+      </c>
+      <c r="G48" s="7" t="inlineStr">
+        <is>
+          <t>Reuters / AGBI</t>
         </is>
       </c>
     </row>
     <row r="49" ht="22" customHeight="1">
       <c r="A49" s="7" t="inlineStr">
         <is>
+          <t>2024-11-01</t>
+        </is>
+      </c>
+      <c r="B49" s="7" t="inlineStr">
+        <is>
+          <t>MGX/Mubadala</t>
+        </is>
+      </c>
+      <c r="C49" s="7" t="inlineStr">
+        <is>
+          <t>Databricks</t>
+        </is>
+      </c>
+      <c r="D49" s="7" t="inlineStr">
+        <is>
+          <t>AI/ML Platform</t>
+        </is>
+      </c>
+      <c r="E49" s="7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F49" s="7" t="inlineStr">
+        <is>
+          <t>Fund ($10B round, $62B val.)</t>
+        </is>
+      </c>
+      <c r="G49" s="7" t="inlineStr">
+        <is>
+          <t>Bloomberg / Global SWF</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="22" customHeight="1">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>2024-11-11</t>
+        </is>
+      </c>
+      <c r="B50" s="6" t="inlineStr">
+        <is>
+          <t>ADIA</t>
+        </is>
+      </c>
+      <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>Qlik Technologies (with Thoma Bravo)</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>AI/ML Platform</t>
+        </is>
+      </c>
+      <c r="E50" s="6" t="inlineStr">
+        <is>
+          <t>US / Sweden</t>
+        </is>
+      </c>
+      <c r="F50" s="6" t="inlineStr">
+        <is>
+          <t>Stake (~$1B minority, $10B val.)</t>
+        </is>
+      </c>
+      <c r="G50" s="6" t="inlineStr">
+        <is>
+          <t>Bloomberg / The National News</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="22" customHeight="1">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>ADIA</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>AlphaGen / ArcLight Capital</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>Power Infrastructure</t>
+        </is>
+      </c>
+      <c r="E51" s="6" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F51" s="6" t="inlineStr">
+        <is>
+          <t>Stake ($500M minority, 11GW)</t>
+        </is>
+      </c>
+      <c r="G51" s="6" t="inlineStr">
+        <is>
+          <t>Reuters / Arab News</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="22" customHeight="1">
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>2025-01-21</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>MGX/Mubadala</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>OpenAI / SoftBank / Oracle (Stargate)</t>
+        </is>
+      </c>
+      <c r="D52" s="7" t="inlineStr">
+        <is>
+          <t>AI Infrastructure</t>
+        </is>
+      </c>
+      <c r="E52" s="7" t="inlineStr">
+        <is>
+          <t>US (Global)</t>
+        </is>
+      </c>
+      <c r="F52" s="7" t="inlineStr">
+        <is>
+          <t>JV ($500B AI infra, $7B MGX equity)</t>
+        </is>
+      </c>
+      <c r="G52" s="7" t="inlineStr">
+        <is>
+          <t>Reuters / Bloomberg / MEI</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" ht="22" customHeight="1">
+      <c r="A53" s="7" t="inlineStr">
+        <is>
+          <t>2025-03-19</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="inlineStr">
+        <is>
+          <t>MGX/Mubadala</t>
+        </is>
+      </c>
+      <c r="C53" s="7" t="inlineStr">
+        <is>
+          <t>NVIDIA / xAI (joined AIP)</t>
+        </is>
+      </c>
+      <c r="D53" s="7" t="inlineStr">
+        <is>
+          <t>AI Infrastructure</t>
+        </is>
+      </c>
+      <c r="E53" s="7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F53" s="7" t="inlineStr">
+        <is>
+          <t>JV (AIP expansion with NVIDIA, xAI)</t>
+        </is>
+      </c>
+      <c r="G53" s="7" t="inlineStr">
+        <is>
+          <t>BlackRock / Bloomberg</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" ht="22" customHeight="1">
+      <c r="A54" s="6" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B54" s="6" t="inlineStr">
+        <is>
+          <t>ADIA</t>
+        </is>
+      </c>
+      <c r="C54" s="6" t="inlineStr">
+        <is>
+          <t>Vantage Data Centers (with GIC)</t>
+        </is>
+      </c>
+      <c r="D54" s="6" t="inlineStr">
+        <is>
+          <t>Data Centers</t>
+        </is>
+      </c>
+      <c r="E54" s="6" t="inlineStr">
+        <is>
+          <t>Asia-Pacific</t>
+        </is>
+      </c>
+      <c r="F54" s="6" t="inlineStr">
+        <is>
+          <t>Fund ($1.6B APAC platform)</t>
+        </is>
+      </c>
+      <c r="G54" s="6" t="inlineStr">
+        <is>
+          <t>Bloomberg / The National News</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="22" customHeight="1">
+      <c r="A55" s="7" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B55" s="7" t="inlineStr">
+        <is>
+          <t>MGX/Mubadala</t>
+        </is>
+      </c>
+      <c r="C55" s="7" t="inlineStr">
+        <is>
+          <t>Altera / Intel (with Silver Lake)</t>
+        </is>
+      </c>
+      <c r="D55" s="7" t="inlineStr">
+        <is>
+          <t>Semiconductors</t>
+        </is>
+      </c>
+      <c r="E55" s="7" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F55" s="7" t="inlineStr">
+        <is>
+          <t>Stake (51% of Altera, $8.75B val.)</t>
+        </is>
+      </c>
+      <c r="G55" s="7" t="inlineStr">
+        <is>
+          <t>Bloomberg / MGX Official</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="22" customHeight="1">
+      <c r="A56" s="7" t="inlineStr">
+        <is>
           <t>2025-10-14</t>
         </is>
       </c>
-      <c r="B49" s="7" t="inlineStr">
+      <c r="B56" s="7" t="inlineStr">
         <is>
           <t>MGX/Mubadala</t>
         </is>
       </c>
-      <c r="C49" s="7" t="inlineStr">
+      <c r="C56" s="7" t="inlineStr">
         <is>
           <t>Aligned Data Centers (via AIP/GIP)</t>
         </is>
       </c>
-      <c r="D49" s="7" t="inlineStr">
+      <c r="D56" s="7" t="inlineStr">
         <is>
           <t>Data Centers</t>
         </is>
       </c>
-      <c r="E49" s="7" t="inlineStr">
+      <c r="E56" s="7" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F49" s="7" t="inlineStr">
+      <c r="F56" s="7" t="inlineStr">
         <is>
           <t>Stake ($40B acquisition, 100% equity)</t>
         </is>
       </c>
-      <c r="G49" s="7" t="inlineStr">
+      <c r="G56" s="7" t="inlineStr">
         <is>
           <t>Bloomberg / BlackRock</t>
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="8" t="inlineStr">
+    <row r="58">
+      <c r="A58" s="8" t="inlineStr">
         <is>
           <t>SUMMARY</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="9" t="inlineStr">
+    <row r="59">
+      <c r="A59" s="9" t="inlineStr">
         <is>
           <t>ADIA</t>
         </is>
       </c>
-      <c r="B52" s="10" t="inlineStr">
-        <is>
-          <t>4 deals</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="9" t="inlineStr">
+      <c r="B59" s="10" t="inlineStr">
+        <is>
+          <t>7 deals</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="9" t="inlineStr">
         <is>
           <t>MGX/Mubadala</t>
         </is>
       </c>
-      <c r="B53" s="10" t="inlineStr">
-        <is>
-          <t>8 deals</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="9" t="inlineStr">
+      <c r="B60" s="10" t="inlineStr">
+        <is>
+          <t>9 deals</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="9" t="inlineStr">
         <is>
           <t>PIF</t>
         </is>
       </c>
-      <c r="B54" s="10" t="inlineStr">
-        <is>
-          <t>20 deals</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="9" t="inlineStr">
+      <c r="B61" s="10" t="inlineStr">
+        <is>
+          <t>23 deals</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="9" t="inlineStr">
         <is>
           <t>QIA</t>
         </is>
       </c>
-      <c r="B55" s="10" t="inlineStr">
+      <c r="B62" s="10" t="inlineStr">
         <is>
           <t>13 deals</t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="11" t="inlineStr">
+    <row r="63">
+      <c r="A63" s="11" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B56" s="11" t="inlineStr">
-        <is>
-          <t>45 deals</t>
+      <c r="B63" s="11" t="inlineStr">
+        <is>
+          <t>52 deals</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G49"/>
+  <autoFilter ref="A4:G56"/>
   <mergeCells count="3">
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A58:G58"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A51:G51"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>